<commit_message>
modify retirement profile HDV
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_CarbonBudget.xlsx
+++ b/SuppXLS/Scen_SYS_CarbonBudget.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bcf850925e8c42cd/Desktop/times-ireland-model/SuppXLS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF5C80B-B865-4109-BB36-F1B41644C5CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{6CF5C80B-B865-4109-BB36-F1B41644C5CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA92EA58-51C1-4E75-8F7C-DFD8F563E907}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="24" r:id="rId1"/>
@@ -1120,7 +1120,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>22860</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -1498,20 +1498,20 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="6" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="10" width="8.140625" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" customWidth="1"/>
+    <col min="1" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="6" width="14.109375" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" customWidth="1"/>
+    <col min="8" max="10" width="8.109375" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" customWidth="1"/>
+    <col min="12" max="12" width="8.109375" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11.44140625" customWidth="1"/>
+    <col min="15" max="15" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="18"/>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -1539,7 +1539,7 @@
       <c r="Y1" s="19"/>
       <c r="Z1" s="19"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -1567,7 +1567,7 @@
       <c r="Y2" s="19"/>
       <c r="Z2" s="19"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="18"/>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -1595,7 +1595,7 @@
       <c r="Y3" s="19"/>
       <c r="Z3" s="19"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="18"/>
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
@@ -1623,7 +1623,7 @@
       <c r="Y4" s="19"/>
       <c r="Z4" s="19"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="18"/>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
@@ -1651,7 +1651,7 @@
       <c r="Y5" s="19"/>
       <c r="Z5" s="19"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="18"/>
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
@@ -1679,7 +1679,7 @@
       <c r="Y6" s="19"/>
       <c r="Z6" s="19"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="18"/>
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
@@ -1707,7 +1707,7 @@
       <c r="Y7" s="19"/>
       <c r="Z7" s="19"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="18"/>
       <c r="B8" s="18"/>
       <c r="C8" s="18"/>
@@ -1735,7 +1735,7 @@
       <c r="Y8" s="19"/>
       <c r="Z8" s="19"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="18"/>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
@@ -1763,7 +1763,7 @@
       <c r="Y9" s="19"/>
       <c r="Z9" s="19"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
@@ -1791,7 +1791,7 @@
       <c r="Y10" s="19"/>
       <c r="Z10" s="19"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
@@ -1819,7 +1819,7 @@
       <c r="Y11" s="19"/>
       <c r="Z11" s="19"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
@@ -1847,7 +1847,7 @@
       <c r="Y12" s="19"/>
       <c r="Z12" s="19"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
@@ -1875,7 +1875,7 @@
       <c r="Y13" s="19"/>
       <c r="Z13" s="19"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
@@ -1903,7 +1903,7 @@
       <c r="Y14" s="19"/>
       <c r="Z14" s="19"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
@@ -1931,7 +1931,7 @@
       <c r="Y15" s="19"/>
       <c r="Z15" s="19"/>
     </row>
-    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="34" t="s">
         <v>91</v>
       </c>
@@ -1961,7 +1961,7 @@
       <c r="Y16" s="19"/>
       <c r="Z16" s="19"/>
     </row>
-    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22"/>
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
@@ -1989,7 +1989,7 @@
       <c r="Y17" s="19"/>
       <c r="Z17" s="19"/>
     </row>
-    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="22"/>
       <c r="B18" s="22"/>
       <c r="C18" s="22"/>
@@ -2017,7 +2017,7 @@
       <c r="Y18" s="19"/>
       <c r="Z18" s="19"/>
     </row>
-    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="25" t="s">
         <v>92</v>
       </c>
@@ -2049,7 +2049,7 @@
       <c r="Y19" s="19"/>
       <c r="Z19" s="19"/>
     </row>
-    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="25" t="s">
         <v>93</v>
       </c>
@@ -2081,7 +2081,7 @@
       <c r="Y20" s="19"/>
       <c r="Z20" s="19"/>
     </row>
-    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="25" t="s">
         <v>94</v>
       </c>
@@ -2113,7 +2113,7 @@
       <c r="Y21" s="19"/>
       <c r="Z21" s="19"/>
     </row>
-    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="25"/>
       <c r="B22" s="28"/>
       <c r="C22" s="28"/>
@@ -2141,7 +2141,7 @@
       <c r="Y22" s="19"/>
       <c r="Z22" s="19"/>
     </row>
-    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="25" t="s">
         <v>95</v>
       </c>
@@ -2173,7 +2173,7 @@
       <c r="Y23" s="19"/>
       <c r="Z23" s="19"/>
     </row>
-    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="25"/>
       <c r="B24" s="28"/>
       <c r="C24" s="28"/>
@@ -2201,7 +2201,7 @@
       <c r="Y24" s="19"/>
       <c r="Z24" s="19"/>
     </row>
-    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="25"/>
       <c r="B25" s="28"/>
       <c r="C25" s="28"/>
@@ -2229,7 +2229,7 @@
       <c r="Y25" s="19"/>
       <c r="Z25" s="19"/>
     </row>
-    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="25" t="s">
         <v>96</v>
       </c>
@@ -2261,7 +2261,7 @@
       <c r="Y26" s="19"/>
       <c r="Z26" s="19"/>
     </row>
-    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="25"/>
       <c r="B27" s="28"/>
       <c r="C27" s="28"/>
@@ -2289,7 +2289,7 @@
       <c r="Y27" s="19"/>
       <c r="Z27" s="19"/>
     </row>
-    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="25"/>
       <c r="B28" s="28"/>
       <c r="C28" s="28"/>
@@ -2317,7 +2317,7 @@
       <c r="Y28" s="19"/>
       <c r="Z28" s="19"/>
     </row>
-    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="25" t="s">
         <v>97</v>
       </c>
@@ -2347,7 +2347,7 @@
       <c r="Y29" s="19"/>
       <c r="Z29" s="19"/>
     </row>
-    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="25" t="s">
         <v>98</v>
       </c>
@@ -2379,7 +2379,7 @@
       <c r="Y30" s="19"/>
       <c r="Z30" s="19"/>
     </row>
-    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="25" t="s">
         <v>100</v>
       </c>
@@ -2411,7 +2411,7 @@
       <c r="Y31" s="19"/>
       <c r="Z31" s="19"/>
     </row>
-    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="31"/>
       <c r="B32" s="32" t="s">
         <v>102</v>
@@ -2441,7 +2441,7 @@
       <c r="Y32" s="19"/>
       <c r="Z32" s="19"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A33" s="18"/>
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
@@ -2469,7 +2469,7 @@
       <c r="Y33" s="19"/>
       <c r="Z33" s="19"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A34" s="18"/>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
@@ -2497,7 +2497,7 @@
       <c r="Y34" s="19"/>
       <c r="Z34" s="19"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A35" s="18"/>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
@@ -2525,7 +2525,7 @@
       <c r="Y35" s="19"/>
       <c r="Z35" s="19"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A36" s="18"/>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
@@ -2553,7 +2553,7 @@
       <c r="Y36" s="19"/>
       <c r="Z36" s="19"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A37" s="18"/>
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
@@ -2581,7 +2581,7 @@
       <c r="Y37" s="19"/>
       <c r="Z37" s="19"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A38" s="18"/>
       <c r="B38" s="18"/>
       <c r="C38" s="18"/>
@@ -2609,7 +2609,7 @@
       <c r="Y38" s="19"/>
       <c r="Z38" s="19"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A39" s="18"/>
       <c r="B39" s="18"/>
       <c r="C39" s="18"/>
@@ -2637,7 +2637,7 @@
       <c r="Y39" s="19"/>
       <c r="Z39" s="19"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A40" s="18"/>
       <c r="B40" s="18"/>
       <c r="C40" s="18"/>
@@ -2665,7 +2665,7 @@
       <c r="Y40" s="19"/>
       <c r="Z40" s="19"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A41" s="18"/>
       <c r="B41" s="18"/>
       <c r="C41" s="18"/>
@@ -2693,7 +2693,7 @@
       <c r="Y41" s="19"/>
       <c r="Z41" s="19"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A42" s="18"/>
       <c r="B42" s="18"/>
       <c r="C42" s="18"/>
@@ -2721,7 +2721,7 @@
       <c r="Y42" s="19"/>
       <c r="Z42" s="19"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A43" s="19"/>
       <c r="B43" s="19"/>
       <c r="C43" s="19"/>
@@ -2749,7 +2749,7 @@
       <c r="Y43" s="19"/>
       <c r="Z43" s="19"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A44" s="19"/>
       <c r="B44" s="19"/>
       <c r="C44" s="19"/>
@@ -2777,7 +2777,7 @@
       <c r="Y44" s="19"/>
       <c r="Z44" s="19"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A45" s="19"/>
       <c r="B45" s="19"/>
       <c r="C45" s="19"/>
@@ -2805,7 +2805,7 @@
       <c r="Y45" s="19"/>
       <c r="Z45" s="19"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A46" s="19"/>
       <c r="B46" s="19"/>
       <c r="C46" s="19"/>
@@ -2833,7 +2833,7 @@
       <c r="Y46" s="19"/>
       <c r="Z46" s="19"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A47" s="19"/>
       <c r="B47" s="19"/>
       <c r="C47" s="19"/>
@@ -2861,7 +2861,7 @@
       <c r="Y47" s="19"/>
       <c r="Z47" s="19"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A48" s="19"/>
       <c r="B48" s="19"/>
       <c r="C48" s="19"/>
@@ -2889,7 +2889,7 @@
       <c r="Y48" s="19"/>
       <c r="Z48" s="19"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A49" s="19"/>
       <c r="B49" s="19"/>
       <c r="C49" s="19"/>
@@ -2917,7 +2917,7 @@
       <c r="Y49" s="19"/>
       <c r="Z49" s="19"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A50" s="19"/>
       <c r="B50" s="19"/>
       <c r="C50" s="19"/>
@@ -2945,7 +2945,7 @@
       <c r="Y50" s="19"/>
       <c r="Z50" s="19"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A51" s="19"/>
       <c r="B51" s="19"/>
       <c r="C51" s="19"/>
@@ -2973,7 +2973,7 @@
       <c r="Y51" s="19"/>
       <c r="Z51" s="19"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A52" s="19"/>
       <c r="B52" s="19"/>
       <c r="C52" s="19"/>
@@ -3001,7 +3001,7 @@
       <c r="Y52" s="19"/>
       <c r="Z52" s="19"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A53" s="19"/>
       <c r="B53" s="19"/>
       <c r="C53" s="19"/>
@@ -3029,7 +3029,7 @@
       <c r="Y53" s="19"/>
       <c r="Z53" s="19"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A54" s="19"/>
       <c r="B54" s="19"/>
       <c r="C54" s="19"/>
@@ -3057,7 +3057,7 @@
       <c r="Y54" s="19"/>
       <c r="Z54" s="19"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A55" s="19"/>
       <c r="B55" s="19"/>
       <c r="C55" s="19"/>
@@ -3085,7 +3085,7 @@
       <c r="Y55" s="19"/>
       <c r="Z55" s="19"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A56" s="19"/>
       <c r="B56" s="19"/>
       <c r="C56" s="19"/>
@@ -3113,7 +3113,7 @@
       <c r="Y56" s="19"/>
       <c r="Z56" s="19"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A57" s="19"/>
       <c r="B57" s="19"/>
       <c r="C57" s="19"/>
@@ -3141,7 +3141,7 @@
       <c r="Y57" s="19"/>
       <c r="Z57" s="19"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A58" s="19"/>
       <c r="B58" s="19"/>
       <c r="C58" s="19"/>
@@ -3169,7 +3169,7 @@
       <c r="Y58" s="19"/>
       <c r="Z58" s="19"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A59" s="19"/>
       <c r="B59" s="19"/>
       <c r="C59" s="19"/>
@@ -3197,7 +3197,7 @@
       <c r="Y59" s="19"/>
       <c r="Z59" s="19"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A60" s="19"/>
       <c r="B60" s="19"/>
       <c r="C60" s="19"/>
@@ -3225,7 +3225,7 @@
       <c r="Y60" s="19"/>
       <c r="Z60" s="19"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A61" s="19"/>
       <c r="B61" s="19"/>
       <c r="C61" s="19"/>
@@ -3253,7 +3253,7 @@
       <c r="Y61" s="19"/>
       <c r="Z61" s="19"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A62" s="19"/>
       <c r="B62" s="19"/>
       <c r="C62" s="19"/>
@@ -3281,7 +3281,7 @@
       <c r="Y62" s="19"/>
       <c r="Z62" s="19"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A63" s="19"/>
       <c r="B63" s="19"/>
       <c r="C63" s="19"/>
@@ -3309,7 +3309,7 @@
       <c r="Y63" s="19"/>
       <c r="Z63" s="19"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A64" s="19"/>
       <c r="B64" s="19"/>
       <c r="C64" s="19"/>
@@ -3337,7 +3337,7 @@
       <c r="Y64" s="19"/>
       <c r="Z64" s="19"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A65" s="19"/>
       <c r="B65" s="19"/>
       <c r="C65" s="19"/>
@@ -3365,7 +3365,7 @@
       <c r="Y65" s="19"/>
       <c r="Z65" s="19"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A66" s="19"/>
       <c r="B66" s="19"/>
       <c r="C66" s="19"/>
@@ -3393,7 +3393,7 @@
       <c r="Y66" s="19"/>
       <c r="Z66" s="19"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A67" s="19"/>
       <c r="B67" s="19"/>
       <c r="C67" s="19"/>
@@ -3421,7 +3421,7 @@
       <c r="Y67" s="19"/>
       <c r="Z67" s="19"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A68" s="19"/>
       <c r="B68" s="19"/>
       <c r="C68" s="19"/>
@@ -3449,7 +3449,7 @@
       <c r="Y68" s="19"/>
       <c r="Z68" s="19"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A69" s="19"/>
       <c r="B69" s="19"/>
       <c r="C69" s="19"/>
@@ -3477,7 +3477,7 @@
       <c r="Y69" s="19"/>
       <c r="Z69" s="19"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A70" s="19"/>
       <c r="B70" s="19"/>
       <c r="C70" s="19"/>
@@ -3505,7 +3505,7 @@
       <c r="Y70" s="19"/>
       <c r="Z70" s="19"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A71" s="19"/>
       <c r="B71" s="19"/>
       <c r="C71" s="19"/>
@@ -3533,7 +3533,7 @@
       <c r="Y71" s="19"/>
       <c r="Z71" s="19"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A72" s="19"/>
       <c r="B72" s="19"/>
       <c r="C72" s="19"/>
@@ -3561,7 +3561,7 @@
       <c r="Y72" s="19"/>
       <c r="Z72" s="19"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A73" s="19"/>
       <c r="B73" s="19"/>
       <c r="C73" s="19"/>
@@ -3589,7 +3589,7 @@
       <c r="Y73" s="19"/>
       <c r="Z73" s="19"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A74" s="19"/>
       <c r="B74" s="19"/>
       <c r="C74" s="19"/>
@@ -3617,7 +3617,7 @@
       <c r="Y74" s="19"/>
       <c r="Z74" s="19"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A75" s="19"/>
       <c r="B75" s="19"/>
       <c r="C75" s="19"/>
@@ -3645,7 +3645,7 @@
       <c r="Y75" s="19"/>
       <c r="Z75" s="19"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A76" s="19"/>
       <c r="B76" s="19"/>
       <c r="C76" s="19"/>
@@ -3673,7 +3673,7 @@
       <c r="Y76" s="19"/>
       <c r="Z76" s="19"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A77" s="19"/>
       <c r="B77" s="19"/>
       <c r="C77" s="19"/>
@@ -3701,7 +3701,7 @@
       <c r="Y77" s="19"/>
       <c r="Z77" s="19"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A78" s="19"/>
       <c r="B78" s="19"/>
       <c r="C78" s="19"/>
@@ -3729,7 +3729,7 @@
       <c r="Y78" s="19"/>
       <c r="Z78" s="19"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A79" s="19"/>
       <c r="B79" s="19"/>
       <c r="C79" s="19"/>
@@ -3757,7 +3757,7 @@
       <c r="Y79" s="19"/>
       <c r="Z79" s="19"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A80" s="19"/>
       <c r="B80" s="19"/>
       <c r="C80" s="19"/>
@@ -3785,7 +3785,7 @@
       <c r="Y80" s="19"/>
       <c r="Z80" s="19"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A81" s="19"/>
       <c r="B81" s="19"/>
       <c r="C81" s="19"/>
@@ -3813,7 +3813,7 @@
       <c r="Y81" s="19"/>
       <c r="Z81" s="19"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A82" s="19"/>
       <c r="B82" s="19"/>
       <c r="C82" s="19"/>
@@ -3841,7 +3841,7 @@
       <c r="Y82" s="19"/>
       <c r="Z82" s="19"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A83" s="19"/>
       <c r="B83" s="19"/>
       <c r="C83" s="19"/>
@@ -3869,7 +3869,7 @@
       <c r="Y83" s="19"/>
       <c r="Z83" s="19"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A84" s="19"/>
       <c r="B84" s="19"/>
       <c r="C84" s="19"/>
@@ -3897,7 +3897,7 @@
       <c r="Y84" s="19"/>
       <c r="Z84" s="19"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A85" s="19"/>
       <c r="B85" s="19"/>
       <c r="C85" s="19"/>
@@ -3925,7 +3925,7 @@
       <c r="Y85" s="19"/>
       <c r="Z85" s="19"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A86" s="19"/>
       <c r="B86" s="19"/>
       <c r="C86" s="19"/>
@@ -3953,7 +3953,7 @@
       <c r="Y86" s="19"/>
       <c r="Z86" s="19"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A87" s="19"/>
       <c r="B87" s="19"/>
       <c r="C87" s="19"/>
@@ -3981,7 +3981,7 @@
       <c r="Y87" s="19"/>
       <c r="Z87" s="19"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A88" s="19"/>
       <c r="B88" s="19"/>
       <c r="C88" s="19"/>
@@ -4009,7 +4009,7 @@
       <c r="Y88" s="19"/>
       <c r="Z88" s="19"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A89" s="19"/>
       <c r="B89" s="19"/>
       <c r="C89" s="19"/>
@@ -4037,7 +4037,7 @@
       <c r="Y89" s="19"/>
       <c r="Z89" s="19"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A90" s="19"/>
       <c r="B90" s="19"/>
       <c r="C90" s="19"/>
@@ -4065,7 +4065,7 @@
       <c r="Y90" s="19"/>
       <c r="Z90" s="19"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A91" s="19"/>
       <c r="B91" s="19"/>
       <c r="C91" s="19"/>
@@ -4093,7 +4093,7 @@
       <c r="Y91" s="19"/>
       <c r="Z91" s="19"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A92" s="19"/>
       <c r="B92" s="19"/>
       <c r="C92" s="19"/>
@@ -4121,7 +4121,7 @@
       <c r="Y92" s="19"/>
       <c r="Z92" s="19"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A93" s="19"/>
       <c r="B93" s="19"/>
       <c r="C93" s="19"/>
@@ -4149,7 +4149,7 @@
       <c r="Y93" s="19"/>
       <c r="Z93" s="19"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A94" s="19"/>
       <c r="B94" s="19"/>
       <c r="C94" s="19"/>
@@ -4177,7 +4177,7 @@
       <c r="Y94" s="19"/>
       <c r="Z94" s="19"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A95" s="19"/>
       <c r="B95" s="19"/>
       <c r="C95" s="19"/>
@@ -4205,7 +4205,7 @@
       <c r="Y95" s="19"/>
       <c r="Z95" s="19"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A96" s="19"/>
       <c r="B96" s="19"/>
       <c r="C96" s="19"/>
@@ -4233,7 +4233,7 @@
       <c r="Y96" s="19"/>
       <c r="Z96" s="19"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A97" s="19"/>
       <c r="B97" s="19"/>
       <c r="C97" s="19"/>
@@ -4261,7 +4261,7 @@
       <c r="Y97" s="19"/>
       <c r="Z97" s="19"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A98" s="19"/>
       <c r="B98" s="19"/>
       <c r="C98" s="19"/>
@@ -4289,7 +4289,7 @@
       <c r="Y98" s="19"/>
       <c r="Z98" s="19"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A99" s="19"/>
       <c r="B99" s="19"/>
       <c r="C99" s="19"/>
@@ -4346,39 +4346,39 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.5703125" customWidth="1"/>
-    <col min="25" max="25" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5546875" customWidth="1"/>
+    <col min="25" max="25" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="6" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="str" cm="1">
         <f t="array" ref="C3">IF(LEFT(INDEX(C5:C7,$A$4),1)&lt;&gt;"*",INDEX(C5:C7,$A$4),"")</f>
         <v>IE</v>
@@ -4492,12 +4492,12 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -4612,7 +4612,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -4729,7 +4729,7 @@
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -4846,7 +4846,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
@@ -4854,7 +4854,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>34</v>
       </c>
@@ -4862,7 +4862,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
@@ -4870,7 +4870,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -4878,7 +4878,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
@@ -4886,7 +4886,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -4894,7 +4894,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>39</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>40</v>
       </c>
@@ -4910,7 +4910,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>41</v>
       </c>
@@ -4918,7 +4918,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>42</v>
       </c>
@@ -4926,7 +4926,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>43</v>
       </c>
@@ -4934,7 +4934,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>44</v>
       </c>
@@ -4942,7 +4942,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>45</v>
       </c>
@@ -4950,7 +4950,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>46</v>
       </c>
@@ -4958,7 +4958,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>47</v>
       </c>
@@ -4966,7 +4966,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>48</v>
       </c>
@@ -4974,7 +4974,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>49</v>
       </c>
@@ -4982,7 +4982,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>50</v>
       </c>
@@ -4990,7 +4990,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>51</v>
       </c>
@@ -4998,7 +4998,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>52</v>
       </c>
@@ -5006,7 +5006,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>53</v>
       </c>
@@ -5014,7 +5014,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>54</v>
       </c>
@@ -5022,7 +5022,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>55</v>
       </c>
@@ -5030,7 +5030,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>56</v>
       </c>
@@ -5038,7 +5038,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>57</v>
       </c>
@@ -5046,7 +5046,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>58</v>
       </c>
@@ -5054,7 +5054,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>59</v>
       </c>
@@ -5062,7 +5062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>60</v>
       </c>
@@ -5088,7 +5088,7 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:colOff>22860</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -5108,22 +5108,22 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B4:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>61</v>
       </c>
@@ -5144,7 +5144,7 @@
         <v>UC_CB_0_Mt_2051-2100</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>68</v>
       </c>
@@ -5165,7 +5165,7 @@
         <v>Carbon budget 0 Mt 2051-2100</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>74</v>
       </c>
@@ -5182,7 +5182,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>69</v>
       </c>
@@ -5201,7 +5201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>82</v>
       </c>
@@ -5218,7 +5218,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>62</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>73</v>
       </c>
@@ -5252,7 +5252,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>77</v>
       </c>
@@ -5269,7 +5269,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>0</v>
       </c>
@@ -5286,7 +5286,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>81</v>
       </c>
@@ -5303,7 +5303,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>76</v>
       </c>
@@ -5331,48 +5331,48 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="str">
         <f>"~UC_Sets: R_E: "  &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3)</f>
         <v>~UC_Sets: R_E: IE</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H4" t="str">
         <f>IF(RIGHT(B2,1)&lt;&gt;" ","~UC_T","")</f>
         <v>~UC_T</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
         <v>61</v>
       </c>
@@ -5407,7 +5407,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>71</v>
       </c>
@@ -5424,7 +5424,7 @@
       </c>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" t="str">
         <f>VLOOKUP($B$5, config!$B$4:$F$14,2,FALSE) &amp; "_Single"</f>
         <v>UC_CB_164_Mt_2021-2025_Single</v>
@@ -5462,7 +5462,7 @@
         <v>Carbon budget 164 Mt 2021-2025 - Single</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C8" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,2,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
@@ -5484,7 +5484,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" t="str">
         <f>VLOOKUP($B$5, config!$B$4:$F$14,3,FALSE) &amp; "_Single"</f>
         <v>UC_CB_112_Mt_2026-2030_Single</v>
@@ -5522,7 +5522,7 @@
         <v>Carbon budget 112 Mt 2026-2030 - Single</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C10" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,3,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
@@ -5544,7 +5544,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" t="str">
         <f>VLOOKUP($B$5, config!$B$4:$F$14,4,FALSE) &amp; "_Single"</f>
         <v>UC_CB_109_Mt_2031-2050_Single</v>
@@ -5582,7 +5582,7 @@
         <v>Carbon budget 109 Mt 2031-2050 - Single</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C12" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,4,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
@@ -5604,7 +5604,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
         <f>VLOOKUP($B$5, config!$B$4:$F$14,5,FALSE) &amp; "_Single"</f>
         <v>UC_CB_0_Mt_2051-2100_Single</v>
@@ -5642,7 +5642,7 @@
         <v>Carbon budget 0 Mt 2051-2100 - Single</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C14" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,5,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
@@ -5679,44 +5679,44 @@
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="str">
         <f>"~UC_Sets: R_S: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!D3:AD3)</f>
         <v>~UC_Sets: R_S: National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H4" t="str">
         <f>IF(RIGHT(B2,1)&lt;&gt;" ","~UC_T","")</f>
         <v>~UC_T</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
         <v>61</v>
       </c>
@@ -5751,7 +5751,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>71</v>
       </c>
@@ -5768,7 +5768,7 @@
       </c>
       <c r="L6" s="7"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" t="str">
         <f>VLOOKUP(B$5, config!$B$4:$F$14,2,FALSE) &amp; "_Multi"</f>
         <v>UC_CB_164_Mt_2021-2025_Multi</v>
@@ -5806,7 +5806,7 @@
         <v>Carbon budget 164 Mt 2021-2025 - Multi</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C8" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,2,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
@@ -5828,7 +5828,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" t="str">
         <f>VLOOKUP(B$5, config!$B$4:$F$14,3,FALSE) &amp; "_Multi"</f>
         <v>UC_CB_112_Mt_2026-2030_Multi</v>
@@ -5866,7 +5866,7 @@
         <v>Carbon budget 112 Mt 2026-2030 - Multi</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C10" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,3,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
@@ -5888,7 +5888,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" t="str">
         <f>VLOOKUP(B$5, config!$B$4:$F$14,4,FALSE) &amp; "_Multi"</f>
         <v>UC_CB_109_Mt_2031-2050_Multi</v>
@@ -5926,7 +5926,7 @@
         <v>Carbon budget 109 Mt 2031-2050 - Multi</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C12" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,4,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
@@ -5948,7 +5948,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
         <f>VLOOKUP(B$5, config!$B$4:$F$14,5,FALSE) &amp; "_Multi"</f>
         <v>UC_CB_0_Mt_2051-2100_Multi</v>
@@ -5986,7 +5986,7 @@
         <v>Carbon budget 0 Mt 2051-2100 - Multi</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C14" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,5,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
@@ -6023,20 +6023,20 @@
       <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="14" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="15" t="s">
         <v>86</v>
       </c>
@@ -6061,7 +6061,7 @@
         <v>National</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C4" s="8" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
Revert Back to old CBs
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_CarbonBudget.xlsx
+++ b/SuppXLS/Scen_SYS_CarbonBudget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33174365-A604-4EEA-8483-EDBB9A2BC1F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462AC10B-C07D-496E-BBA3-68BD61AE2482}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="24" r:id="rId1"/>
@@ -5108,7 +5108,7 @@
   <dimension ref="B4:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5128,15 +5128,15 @@
       </c>
       <c r="C4" t="str">
         <f xml:space="preserve"> _xlfn.TEXTJOIN("_",TRUE,"UC","CB",ROUND(C7,0),"Mt",C6)</f>
-        <v>UC_CB_295_Mt_2021-2025</v>
+        <v>UC_CB_164_Mt_2021-2025</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" ref="D4:E4" si="0" xml:space="preserve"> _xlfn.TEXTJOIN("_",TRUE,"UC","CB",ROUND(D7,0),"Mt",D6)</f>
-        <v>UC_CB_200_Mt_2026-2030</v>
+        <v>UC_CB_112_Mt_2026-2030</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v>UC_CB_151_Mt_2031-2050</v>
+        <v>UC_CB_109_Mt_2031-2050</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" ref="F4" si="1" xml:space="preserve"> _xlfn.TEXTJOIN("_",TRUE,"UC","CB",ROUND(F7,0),"Mt",F6)</f>
@@ -5149,15 +5149,15 @@
       </c>
       <c r="C5" t="str">
         <f xml:space="preserve"> _xlfn.TEXTJOIN(" ",TRUE,"Carbon budget",ROUND(C7,0),"Mt",C6)</f>
-        <v>Carbon budget 295 Mt 2021-2025</v>
+        <v>Carbon budget 164 Mt 2021-2025</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" ref="D5:F5" si="2" xml:space="preserve"> _xlfn.TEXTJOIN(" ",TRUE,"Carbon budget",ROUND(D7,0),"Mt",D6)</f>
-        <v>Carbon budget 200 Mt 2026-2030</v>
+        <v>Carbon budget 112 Mt 2026-2030</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="2"/>
-        <v>Carbon budget 151 Mt 2031-2050</v>
+        <v>Carbon budget 109 Mt 2031-2050</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="2"/>
@@ -5186,13 +5186,15 @@
         <v>69</v>
       </c>
       <c r="C7">
-        <v>295</v>
+        <f>160+3.5</f>
+        <v>163.5</v>
       </c>
       <c r="D7">
-        <v>200</v>
+        <f>109+2.5</f>
+        <v>111.5</v>
       </c>
       <c r="E7">
-        <v>151</v>
+        <v>109</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -5424,7 +5426,7 @@
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" t="str">
         <f>VLOOKUP($B$5, config!$B$4:$F$14,2,FALSE) &amp; "_Single"</f>
-        <v>UC_CB_295_Mt_2021-2025_Single</v>
+        <v>UC_CB_164_Mt_2021-2025_Single</v>
       </c>
       <c r="C7" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,2,FALSE)</f>
@@ -5452,11 +5454,11 @@
       </c>
       <c r="K7">
         <f>VLOOKUP("Value", config!$B$4:$F$14,2,FALSE)*1000</f>
-        <v>295000</v>
+        <v>163500</v>
       </c>
       <c r="L7" t="str">
         <f>VLOOKUP($L$5, config!$B$4:$F$14,2,FALSE) &amp; " - Single"</f>
-        <v>Carbon budget 295 Mt 2021-2025 - Single</v>
+        <v>Carbon budget 164 Mt 2021-2025 - Single</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -5484,7 +5486,7 @@
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" t="str">
         <f>VLOOKUP($B$5, config!$B$4:$F$14,3,FALSE) &amp; "_Single"</f>
-        <v>UC_CB_200_Mt_2026-2030_Single</v>
+        <v>UC_CB_112_Mt_2026-2030_Single</v>
       </c>
       <c r="C9" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,3,FALSE)</f>
@@ -5512,11 +5514,11 @@
       </c>
       <c r="K9">
         <f>VLOOKUP("Value", config!$B$4:$F$14,3,FALSE)*1000</f>
-        <v>200000</v>
+        <v>111500</v>
       </c>
       <c r="L9" t="str">
         <f>VLOOKUP($L$5, config!$B$4:$F$14,3,FALSE) &amp; " - Single"</f>
-        <v>Carbon budget 200 Mt 2026-2030 - Single</v>
+        <v>Carbon budget 112 Mt 2026-2030 - Single</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -5544,7 +5546,7 @@
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <f>VLOOKUP($B$5, config!$B$4:$F$14,4,FALSE) &amp; "_Single"</f>
-        <v>UC_CB_151_Mt_2031-2050_Single</v>
+        <v>UC_CB_109_Mt_2031-2050_Single</v>
       </c>
       <c r="C11" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,4,FALSE)</f>
@@ -5572,11 +5574,11 @@
       </c>
       <c r="K11">
         <f>VLOOKUP("Value", config!$B$4:$F$14,4,FALSE)*1000</f>
-        <v>151000</v>
+        <v>109000</v>
       </c>
       <c r="L11" t="str">
         <f>VLOOKUP($L$5, config!$B$4:$F$14,4,FALSE) &amp; " - Single"</f>
-        <v>Carbon budget 151 Mt 2031-2050 - Single</v>
+        <v>Carbon budget 109 Mt 2031-2050 - Single</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -5673,7 +5675,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5768,7 +5770,7 @@
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" t="str">
         <f>VLOOKUP(B$5, config!$B$4:$F$14,2,FALSE) &amp; "_Multi"</f>
-        <v>UC_CB_295_Mt_2021-2025_Multi</v>
+        <v>UC_CB_164_Mt_2021-2025_Multi</v>
       </c>
       <c r="C7" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,2,FALSE)</f>
@@ -5796,11 +5798,11 @@
       </c>
       <c r="K7">
         <f>VLOOKUP("Value", config!$B$4:$F$14,2,FALSE)*1000</f>
-        <v>295000</v>
+        <v>163500</v>
       </c>
       <c r="L7" t="str">
         <f>VLOOKUP(L$5, config!$B$4:$F$14,2,FALSE) &amp; " - Multi"</f>
-        <v>Carbon budget 295 Mt 2021-2025 - Multi</v>
+        <v>Carbon budget 164 Mt 2021-2025 - Multi</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -5828,7 +5830,7 @@
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" t="str">
         <f>VLOOKUP(B$5, config!$B$4:$F$14,3,FALSE) &amp; "_Multi"</f>
-        <v>UC_CB_200_Mt_2026-2030_Multi</v>
+        <v>UC_CB_112_Mt_2026-2030_Multi</v>
       </c>
       <c r="C9" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,3,FALSE)</f>
@@ -5856,11 +5858,11 @@
       </c>
       <c r="K9">
         <f>VLOOKUP("Value", config!$B$4:$F$14,3,FALSE)*1000</f>
-        <v>200000</v>
+        <v>111500</v>
       </c>
       <c r="L9" t="str">
         <f>VLOOKUP(L$5, config!$B$4:$F$14,3,FALSE) &amp; " - Multi"</f>
-        <v>Carbon budget 200 Mt 2026-2030 - Multi</v>
+        <v>Carbon budget 112 Mt 2026-2030 - Multi</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -5888,7 +5890,7 @@
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <f>VLOOKUP(B$5, config!$B$4:$F$14,4,FALSE) &amp; "_Multi"</f>
-        <v>UC_CB_151_Mt_2031-2050_Multi</v>
+        <v>UC_CB_109_Mt_2031-2050_Multi</v>
       </c>
       <c r="C11" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,4,FALSE)</f>
@@ -5916,11 +5918,11 @@
       </c>
       <c r="K11">
         <f>VLOOKUP("Value", config!$B$4:$F$14,4,FALSE)*1000</f>
-        <v>151000</v>
+        <v>109000</v>
       </c>
       <c r="L11" t="str">
         <f>VLOOKUP(L$5, config!$B$4:$F$14,4,FALSE) &amp; " - Multi"</f>
-        <v>Carbon budget 151 Mt 2031-2050 - Multi</v>
+        <v>Carbon budget 109 Mt 2031-2050 - Multi</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>